<commit_message>
Updated results and notebooks
</commit_message>
<xml_diff>
--- a/table_results_research_project.xlsx
+++ b/table_results_research_project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aramosvela\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aramosvela\Documents\Research_Project\Research_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5A96AF-58FE-411F-BB83-4E8400841232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCB1749-0665-4554-B1F0-1DB4AE510EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-67308" yWindow="-108" windowWidth="29016" windowHeight="15816" xr2:uid="{483AEDE7-AB78-4168-9B80-55876B051647}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="26">
   <si>
     <t>Model</t>
   </si>
@@ -90,13 +90,37 @@
   </si>
   <si>
     <t>(Higher number of epochs make models overfit)</t>
+  </si>
+  <si>
+    <t>Second experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trained on the same data </t>
+  </si>
+  <si>
+    <t>Inference</t>
+  </si>
+  <si>
+    <t>Generated responses</t>
+  </si>
+  <si>
+    <t>(window=5)</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>GPT2_DialoGPT</t>
+  </si>
+  <si>
+    <t>First experiment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,13 +136,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -148,12 +198,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AA526-AA38-41A9-8CE6-AF1528BBF0C6}">
-  <dimension ref="B2:K23"/>
+  <dimension ref="B1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +537,35 @@
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="N1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="7"/>
+      <c r="P1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+    </row>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -493,12 +578,26 @@
       <c r="E2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,8 +628,38 @@
       <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -561,8 +690,38 @@
       <c r="K5" s="2">
         <v>12.883484299978999</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.96481054104310404</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.117929350867173</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1.78390152851935E-2</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.10578630046257401</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0.105751189202618</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0.86580065354353597</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.85965373864612704</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.86243079912113896</v>
+      </c>
+      <c r="W5" s="2">
+        <v>13.0806181606593</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -593,8 +752,38 @@
       <c r="K6" s="3">
         <v>12.3689070624488</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1.07151119334455</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0.13008312320492901</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>2.7754701993507502E-2</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0.11969950718074</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0.11991817826411599</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0.86969205516355996</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0.85988015217411795</v>
+      </c>
+      <c r="V6" s="5">
+        <v>0.86447452160913396</v>
+      </c>
+      <c r="W6" s="3">
+        <v>11.921884076534701</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -607,8 +796,38 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2.1163319284686501</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.16698830029414699</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>5.6018697670470997E-2</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0.15705717179600101</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.15725250072049099</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0.87986522153705504</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.86395247125063601</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0.87156481570935196</v>
+      </c>
+      <c r="W7" s="3">
+        <v>12.070922004120201</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -621,12 +840,26 @@
       <c r="E9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
@@ -657,8 +890,38 @@
       <c r="K11" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
@@ -689,54 +952,177 @@
       <c r="K12" s="2">
         <v>13.0864931336151</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.37614680912746501</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0.106433625817177</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>8.0658678505576807E-3</v>
+      </c>
+      <c r="R12" s="3">
+        <v>9.0746712040812999E-2</v>
+      </c>
+      <c r="S12" s="3">
+        <v>9.0306512341550904E-2</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0.84216689446876702</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0.84267965644255405</v>
+      </c>
+      <c r="V12" s="3">
+        <v>0.84213208056044297</v>
+      </c>
+      <c r="W12" s="2">
+        <v>11.5638913207681</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="5">
         <v>0.86843254960723404</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="5">
         <v>0.118422070367508</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="5">
         <v>2.1267182416081401E-2</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="5">
         <v>0.107387899518553</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="5">
         <v>0.107542324653501</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="5">
         <v>0.86752158086573905</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="5">
         <v>0.85871535144553002</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="5">
         <v>0.86281287563255504</v>
       </c>
       <c r="K13" s="3">
         <v>12.4539773431901</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="5">
+        <v>0.38246335370461898</v>
+      </c>
+      <c r="P13" s="5">
+        <v>0.103122476889645</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>9.0687640060689908E-3</v>
+      </c>
+      <c r="R13" s="5">
+        <v>9.2723965003074907E-2</v>
+      </c>
+      <c r="S13" s="5">
+        <v>9.2466142549619199E-2</v>
+      </c>
+      <c r="T13" s="5">
+        <v>0.86070055694415604</v>
+      </c>
+      <c r="U13" s="5">
+        <v>0.85028196648619603</v>
+      </c>
+      <c r="V13" s="5">
+        <v>0.855154600636712</v>
+      </c>
+      <c r="W13" s="3">
+        <v>10.9870207983607</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C14" s="2">
+        <v>1.93450592442832</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.16372543693354299</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5.63627733103403E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.154892158578641</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.15524534472924201</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.88236651031925395</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.86225521373828995</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.87188218743043799</v>
+      </c>
+      <c r="K14" s="3">
+        <v>11.150382330231899</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.77776484261849099</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0.12538659964780099</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1.2817914276200101E-2</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0.114838890145729</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0.114761439108219</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0.86947400748044501</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0.855805803646986</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0.86244411475356897</v>
+      </c>
+      <c r="W14" s="3">
+        <v>10.6162901845933</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>22</v>
+      </c>
+      <c r="R17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
@@ -752,12 +1138,24 @@
       <c r="F18" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N19" t="s">
+        <v>15</v>
+      </c>
+      <c r="P19">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
@@ -789,7 +1187,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>1</v>
       </c>
@@ -820,12 +1218,18 @@
       <c r="K21" s="3">
         <v>13.2445610287687</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="5">
         <v>0.877586053702059</v>
       </c>
       <c r="D22" s="2">
@@ -837,35 +1241,73 @@
       <c r="F22" s="2">
         <v>0.110583184502593</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="5">
         <v>0.1104193368921</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="5">
         <v>0.86260821446469704</v>
       </c>
       <c r="I22" s="2">
         <v>0.85617976424134801</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="5">
         <v>0.85920716411292297</v>
       </c>
       <c r="K22" s="2">
         <v>13.2870373577408</v>
       </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N22" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="C23" s="2">
+        <v>0.88540889745921103</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.12249132196028401</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1.22715766680133E-2</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.110388947997518</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.11079447373202</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.86756437366036099</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.85580054131047401</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.86147690984024305</v>
+      </c>
+      <c r="K23" s="3">
+        <v>11.1618913981708</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="N24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P24" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>